<commit_message>
ban may cho viet + lay may 7490
</commit_message>
<xml_diff>
--- a/BanLaptop/NhapXuatLaptop.xlsx
+++ b/BanLaptop/NhapXuatLaptop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04.Private\BanLaptop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32DC02E-9434-464D-B500-2B2D57414540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04D7403-FDEB-4BC1-B902-980FEB14009A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="100">
   <si>
     <t>ID máy</t>
   </si>
@@ -324,6 +324,12 @@
   </si>
   <si>
     <t>Nam /Đạt</t>
+  </si>
+  <si>
+    <t>FW7Q1Z2</t>
+  </si>
+  <si>
+    <t>Việt</t>
   </si>
 </sst>
 </file>
@@ -430,7 +436,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -509,18 +515,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -812,11 +813,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I46" sqref="I46"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +909,7 @@
         <v>6700000</v>
       </c>
       <c r="G2" s="7">
-        <f>(F2*25%)+F2</f>
+        <f t="shared" ref="G2:G17" si="0">(F2*25%)+F2</f>
         <v>8375000</v>
       </c>
       <c r="H2" s="7">
@@ -948,11 +949,11 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7">
-        <f t="shared" ref="F3:F39" si="0">C3+D3+E3</f>
+        <f t="shared" ref="F3:F39" si="1">C3+D3+E3</f>
         <v>6500000</v>
       </c>
       <c r="G3" s="7">
-        <f>(F3*25%)+F3</f>
+        <f t="shared" si="0"/>
         <v>8125000</v>
       </c>
       <c r="H3" s="7">
@@ -962,7 +963,7 @@
         <v>5000</v>
       </c>
       <c r="J3" s="7">
-        <f t="shared" ref="J3:J17" si="1">H3-I3-F3</f>
+        <f t="shared" ref="J3:J17" si="2">H3-I3-F3</f>
         <v>745000</v>
       </c>
       <c r="K3" s="6" t="s">
@@ -992,11 +993,11 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7">
+        <f t="shared" si="1"/>
+        <v>4900000</v>
+      </c>
+      <c r="G4" s="7">
         <f t="shared" si="0"/>
-        <v>4900000</v>
-      </c>
-      <c r="G4" s="7">
-        <f>(F4*25%)+F4</f>
         <v>6125000</v>
       </c>
       <c r="H4" s="7">
@@ -1004,7 +1005,7 @@
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>500000</v>
       </c>
       <c r="K4" s="6" t="s">
@@ -1036,11 +1037,11 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7">
+        <f t="shared" si="1"/>
+        <v>6700000</v>
+      </c>
+      <c r="G5" s="7">
         <f t="shared" si="0"/>
-        <v>6700000</v>
-      </c>
-      <c r="G5" s="7">
-        <f>(F5*25%)+F5</f>
         <v>8375000</v>
       </c>
       <c r="H5" s="7">
@@ -1050,7 +1051,7 @@
         <v>420000</v>
       </c>
       <c r="J5" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>480000</v>
       </c>
       <c r="K5" s="6" t="s">
@@ -1082,11 +1083,11 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7">
+        <f t="shared" si="1"/>
+        <v>7150000</v>
+      </c>
+      <c r="G6" s="7">
         <f t="shared" si="0"/>
-        <v>7150000</v>
-      </c>
-      <c r="G6" s="7">
-        <f>(F6*25%)+F6</f>
         <v>8937500</v>
       </c>
       <c r="H6" s="7">
@@ -1094,7 +1095,7 @@
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>350000</v>
       </c>
       <c r="K6" s="6" t="s">
@@ -1124,11 +1125,11 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7">
+        <f t="shared" si="1"/>
+        <v>7500000</v>
+      </c>
+      <c r="G7" s="7">
         <f t="shared" si="0"/>
-        <v>7500000</v>
-      </c>
-      <c r="G7" s="7">
-        <f>(F7*25%)+F7</f>
         <v>9375000</v>
       </c>
       <c r="H7" s="7">
@@ -1138,7 +1139,7 @@
         <v>10000</v>
       </c>
       <c r="J7" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-10000</v>
       </c>
       <c r="K7" s="6" t="s">
@@ -1168,11 +1169,11 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7">
+        <f t="shared" si="1"/>
+        <v>6700000</v>
+      </c>
+      <c r="G8" s="7">
         <f t="shared" si="0"/>
-        <v>6700000</v>
-      </c>
-      <c r="G8" s="7">
-        <f>(F8*25%)+F8</f>
         <v>8375000</v>
       </c>
       <c r="H8" s="7">
@@ -1182,7 +1183,7 @@
         <v>10000</v>
       </c>
       <c r="J8" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>640000</v>
       </c>
       <c r="K8" s="6" t="s">
@@ -1212,11 +1213,11 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7">
+        <f t="shared" si="1"/>
+        <v>11500000</v>
+      </c>
+      <c r="G9" s="7">
         <f t="shared" si="0"/>
-        <v>11500000</v>
-      </c>
-      <c r="G9" s="7">
-        <f>(F9*25%)+F9</f>
         <v>14375000</v>
       </c>
       <c r="H9" s="7">
@@ -1224,7 +1225,7 @@
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>500000</v>
       </c>
       <c r="K9" s="6" t="s">
@@ -1256,11 +1257,11 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7">
+        <f t="shared" si="1"/>
+        <v>6500000</v>
+      </c>
+      <c r="G10" s="7">
         <f t="shared" si="0"/>
-        <v>6500000</v>
-      </c>
-      <c r="G10" s="7">
-        <f>(F10*25%)+F10</f>
         <v>8125000</v>
       </c>
       <c r="H10" s="7">
@@ -1268,7 +1269,7 @@
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1000000</v>
       </c>
       <c r="K10" s="6" t="s">
@@ -1296,11 +1297,11 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7">
+        <f t="shared" si="1"/>
+        <v>6500000</v>
+      </c>
+      <c r="G11" s="7">
         <f t="shared" si="0"/>
-        <v>6500000</v>
-      </c>
-      <c r="G11" s="7">
-        <f>(F11*25%)+F11</f>
         <v>8125000</v>
       </c>
       <c r="H11" s="7">
@@ -1310,7 +1311,7 @@
         <v>100000</v>
       </c>
       <c r="J11" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>300000</v>
       </c>
       <c r="K11" s="6" t="s">
@@ -1340,11 +1341,11 @@
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7">
+        <f t="shared" si="1"/>
+        <v>5000000</v>
+      </c>
+      <c r="G12" s="7">
         <f t="shared" si="0"/>
-        <v>5000000</v>
-      </c>
-      <c r="G12" s="7">
-        <f>(F12*25%)+F12</f>
         <v>6250000</v>
       </c>
       <c r="H12" s="7">
@@ -1354,7 +1355,7 @@
         <v>5000</v>
       </c>
       <c r="J12" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>795000</v>
       </c>
       <c r="K12" s="6" t="s">
@@ -1386,11 +1387,11 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7">
+        <f t="shared" si="1"/>
+        <v>5500000</v>
+      </c>
+      <c r="G13" s="7">
         <f t="shared" si="0"/>
-        <v>5500000</v>
-      </c>
-      <c r="G13" s="7">
-        <f>(F13*25%)+F13</f>
         <v>6875000</v>
       </c>
       <c r="H13" s="7">
@@ -1398,7 +1399,7 @@
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>800000</v>
       </c>
       <c r="K13" s="6" t="s">
@@ -1430,11 +1431,11 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7">
+        <f t="shared" si="1"/>
+        <v>5500000</v>
+      </c>
+      <c r="G14" s="7">
         <f t="shared" si="0"/>
-        <v>5500000</v>
-      </c>
-      <c r="G14" s="7">
-        <f>(F14*25%)+F14</f>
         <v>6875000</v>
       </c>
       <c r="H14" s="7">
@@ -1442,7 +1443,7 @@
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1100000</v>
       </c>
       <c r="K14" s="6" t="s">
@@ -1472,11 +1473,11 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7">
+        <f t="shared" si="1"/>
+        <v>5700000</v>
+      </c>
+      <c r="G15" s="7">
         <f t="shared" si="0"/>
-        <v>5700000</v>
-      </c>
-      <c r="G15" s="7">
-        <f>(F15*25%)+F15</f>
         <v>7125000</v>
       </c>
       <c r="H15" s="7">
@@ -1484,7 +1485,7 @@
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>500000</v>
       </c>
       <c r="K15" s="6" t="s">
@@ -1516,11 +1517,11 @@
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7">
+        <f t="shared" si="1"/>
+        <v>8000000</v>
+      </c>
+      <c r="G16" s="7">
         <f t="shared" si="0"/>
-        <v>8000000</v>
-      </c>
-      <c r="G16" s="7">
-        <f>(F16*25%)+F16</f>
         <v>10000000</v>
       </c>
       <c r="H16" s="7">
@@ -1528,7 +1529,7 @@
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2500000</v>
       </c>
       <c r="K16" s="6" t="s">
@@ -1556,11 +1557,11 @@
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7">
+        <f t="shared" si="1"/>
+        <v>10835587</v>
+      </c>
+      <c r="G17" s="7">
         <f t="shared" si="0"/>
-        <v>10835587</v>
-      </c>
-      <c r="G17" s="7">
-        <f>(F17*25%)+F17</f>
         <v>13544483.75</v>
       </c>
       <c r="H17" s="7">
@@ -1568,7 +1569,7 @@
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3164413</v>
       </c>
       <c r="K17" s="6" t="s">
@@ -1594,11 +1595,11 @@
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5000000</v>
       </c>
       <c r="G18" s="7">
-        <f t="shared" ref="G18" si="2">(F18*25%)+F18</f>
+        <f t="shared" ref="G18" si="3">(F18*25%)+F18</f>
         <v>6250000</v>
       </c>
       <c r="H18" s="7">
@@ -1606,7 +1607,7 @@
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7">
-        <f t="shared" ref="J18:J44" si="3">H18-I18-F18</f>
+        <f t="shared" ref="J18:J44" si="4">H18-I18-F18</f>
         <v>500000</v>
       </c>
       <c r="K18" s="6" t="s">
@@ -1638,11 +1639,11 @@
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4500000</v>
       </c>
       <c r="G19" s="7">
-        <f t="shared" ref="G19" si="4">(F19*25%)+F19</f>
+        <f t="shared" ref="G19" si="5">(F19*25%)+F19</f>
         <v>5625000</v>
       </c>
       <c r="H19" s="7">
@@ -1650,7 +1651,7 @@
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
       <c r="K19" s="6" t="s">
@@ -1682,11 +1683,11 @@
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7983890</v>
       </c>
       <c r="G20" s="16">
-        <f t="shared" ref="G20:G35" si="5">(F20*25%)+F20</f>
+        <f t="shared" ref="G20:G35" si="6">(F20*25%)+F20</f>
         <v>9979862.5</v>
       </c>
       <c r="H20" s="16">
@@ -1696,7 +1697,7 @@
         <v>50000</v>
       </c>
       <c r="J20" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1466110</v>
       </c>
       <c r="K20" s="6" t="s">
@@ -1730,11 +1731,11 @@
         <v>300000</v>
       </c>
       <c r="F21" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9248805</v>
       </c>
       <c r="G21" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11561006.25</v>
       </c>
       <c r="H21" s="7">
@@ -1744,7 +1745,7 @@
         <v>1500000</v>
       </c>
       <c r="J21" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1251195</v>
       </c>
       <c r="K21" s="6" t="s">
@@ -1778,11 +1779,11 @@
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10561005</v>
       </c>
       <c r="G22" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13201256.25</v>
       </c>
       <c r="H22" s="7">
@@ -1792,7 +1793,7 @@
         <v>900000</v>
       </c>
       <c r="J22" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>538995</v>
       </c>
       <c r="K22" s="6" t="s">
@@ -1819,7 +1820,8 @@
         <v>64</v>
       </c>
       <c r="C23" s="7">
-        <v>5182073</v>
+        <f>5182073+150000</f>
+        <v>5332073</v>
       </c>
       <c r="D23" s="7">
         <v>1375000</v>
@@ -1829,19 +1831,23 @@
       </c>
       <c r="F23" s="7">
         <f>C23+D23+E23</f>
-        <v>5557073</v>
+        <v>5707073</v>
       </c>
       <c r="G23" s="7">
         <f>(F23*25%)+F23</f>
-        <v>6946341.25</v>
-      </c>
-      <c r="H23" s="7"/>
+        <v>7133841.25</v>
+      </c>
+      <c r="H23" s="7">
+        <v>8200000</v>
+      </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7">
-        <f t="shared" si="3"/>
-        <v>-5557073</v>
-      </c>
-      <c r="K23" s="6"/>
+        <f t="shared" si="4"/>
+        <v>2492927</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="L23" s="6"/>
       <c r="M23" s="6" t="s">
         <v>86</v>
@@ -1872,11 +1878,11 @@
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4356172</v>
       </c>
       <c r="G24" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5445215</v>
       </c>
       <c r="H24" s="7">
@@ -1884,7 +1890,7 @@
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2043828</v>
       </c>
       <c r="K24" s="6" t="s">
@@ -1916,24 +1922,32 @@
       <c r="D25" s="7">
         <v>1075000</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="7">
+        <v>490000</v>
+      </c>
       <c r="F25" s="7">
-        <f t="shared" si="0"/>
-        <v>5568148</v>
+        <f t="shared" si="1"/>
+        <v>6058148</v>
       </c>
       <c r="G25" s="7">
-        <f t="shared" si="5"/>
-        <v>6960185</v>
-      </c>
-      <c r="H25" s="7"/>
+        <f t="shared" si="6"/>
+        <v>7572685</v>
+      </c>
+      <c r="H25" s="7">
+        <v>8000000</v>
+      </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7">
-        <f t="shared" si="3"/>
-        <v>-5568148</v>
-      </c>
-      <c r="K25" s="6"/>
+        <f t="shared" si="4"/>
+        <v>1941852</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>50</v>
+      </c>
       <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
+      <c r="M25" s="6" t="s">
+        <v>98</v>
+      </c>
       <c r="N25" s="21" t="s">
         <v>68</v>
       </c>
@@ -1960,11 +1974,11 @@
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4876801</v>
       </c>
       <c r="G26" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6096001.25</v>
       </c>
       <c r="H26" s="7">
@@ -1972,7 +1986,7 @@
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3073199</v>
       </c>
       <c r="K26" s="6" t="s">
@@ -2004,22 +2018,24 @@
       <c r="D27" s="7">
         <v>1050000</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="7">
+        <v>200000</v>
+      </c>
       <c r="F27" s="7">
-        <f t="shared" si="0"/>
-        <v>7587888</v>
+        <f t="shared" si="1"/>
+        <v>7787888</v>
       </c>
       <c r="G27" s="7">
-        <f t="shared" si="5"/>
-        <v>9484860</v>
+        <f t="shared" si="6"/>
+        <v>9734860</v>
       </c>
       <c r="H27" s="7">
         <v>9500000</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="7">
-        <f t="shared" si="3"/>
-        <v>1912112</v>
+        <f t="shared" si="4"/>
+        <v>1712112</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>92</v>
@@ -2052,17 +2068,17 @@
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7887859</v>
       </c>
       <c r="G28" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9859823.75</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-7887859</v>
       </c>
       <c r="K28" s="6"/>
@@ -2092,17 +2108,17 @@
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4850950</v>
       </c>
       <c r="G29" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6063687.5</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-4850950</v>
       </c>
       <c r="K29" s="6"/>
@@ -2132,17 +2148,17 @@
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8317935</v>
       </c>
       <c r="G30" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10397418.75</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-8317935</v>
       </c>
       <c r="K30" s="6"/>
@@ -2169,21 +2185,25 @@
       <c r="C31" s="7">
         <v>4258422</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
+      <c r="D31" s="7">
+        <v>1064000</v>
+      </c>
+      <c r="E31" s="7">
+        <v>-1000000</v>
+      </c>
       <c r="F31" s="7">
-        <f t="shared" si="0"/>
-        <v>4258422</v>
+        <f t="shared" si="1"/>
+        <v>4322422</v>
       </c>
       <c r="G31" s="7">
-        <f t="shared" si="5"/>
-        <v>5323027.5</v>
+        <f t="shared" si="6"/>
+        <v>5403027.5</v>
       </c>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7">
-        <f t="shared" si="3"/>
-        <v>-4258422</v>
+        <f t="shared" si="4"/>
+        <v>-4322422</v>
       </c>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
@@ -2212,17 +2232,17 @@
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6651048</v>
       </c>
       <c r="G32" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8313810</v>
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
       <c r="J32" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-6651048</v>
       </c>
       <c r="K32" s="6"/>
@@ -2252,17 +2272,17 @@
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3558942</v>
       </c>
       <c r="G33" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4448677.5</v>
       </c>
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-3558942</v>
       </c>
       <c r="K33" s="6"/>
@@ -2292,17 +2312,17 @@
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9299103</v>
       </c>
       <c r="G34" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11623878.75</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-9299103</v>
       </c>
       <c r="K34" s="6"/>
@@ -2330,17 +2350,17 @@
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7849892</v>
       </c>
       <c r="G35" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9812365</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-7849892</v>
       </c>
       <c r="K35" s="6"/>
@@ -2370,14 +2390,14 @@
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3972000</v>
       </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
       <c r="J36" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-3972000</v>
       </c>
       <c r="K36" s="6"/>
@@ -2401,14 +2421,14 @@
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8467000</v>
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>-8467000</v>
       </c>
       <c r="K37" s="6"/>
@@ -2428,14 +2448,14 @@
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K38" s="6"/>
@@ -2455,14 +2475,14 @@
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
       <c r="J39" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K39" s="6"/>
@@ -2477,66 +2497,30 @@
       <c r="A40" s="36">
         <v>39</v>
       </c>
-      <c r="B40" s="40"/>
-      <c r="C40" s="41"/>
-      <c r="D40" s="42"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="42"/>
+      <c r="C40" s="40"/>
       <c r="J40" s="7"/>
-      <c r="K40" s="43"/>
-      <c r="L40" s="43"/>
-      <c r="M40" s="43"/>
-      <c r="N40" s="44"/>
-      <c r="O40" s="43"/>
-      <c r="P40" s="45"/>
-      <c r="Q40" s="43"/>
+      <c r="N40" s="41"/>
+      <c r="P40" s="42"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="36">
         <v>40</v>
       </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="42"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
+      <c r="C41" s="40"/>
       <c r="J41" s="7"/>
-      <c r="K41" s="43"/>
-      <c r="L41" s="43"/>
-      <c r="M41" s="43"/>
-      <c r="N41" s="44"/>
-      <c r="O41" s="43"/>
-      <c r="P41" s="45"/>
-      <c r="Q41" s="43"/>
+      <c r="N41" s="41"/>
+      <c r="P41" s="42"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="36"/>
-      <c r="B42" s="40"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="42"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
+      <c r="C42" s="40"/>
       <c r="J42" s="7"/>
-      <c r="K42" s="43"/>
-      <c r="L42" s="43"/>
-      <c r="M42" s="43"/>
-      <c r="N42" s="44"/>
-      <c r="O42" s="43"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="43"/>
+      <c r="N42" s="41"/>
+      <c r="P42" s="42"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="J43" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -2550,7 +2534,7 @@
         <v>50200000</v>
       </c>
       <c r="J44" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50200000</v>
       </c>
       <c r="L44" t="s">
@@ -2560,12 +2544,12 @@
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D48" s="3">
         <f>SUM(C20:C25)</f>
-        <v>37151557</v>
+        <v>37301557</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="K1:K48" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="N26:P26 O26:O42 D26:E42 C29:E38 N29:P38 O23:P25 B2:B25 N2:P22 C2:F2 Q2:Q42 C3:E25 F3:F42 G2:M17 G18:I42 K18:M42 J3:J44">
+  <conditionalFormatting sqref="C2:F2 G2:M17 N2:P22 B2:B25 Q2:Q42 C3:E25 F3:F42 J3:J44 G18:I42 K18:M42 O23:P25 N26:P26 D26:E42 O26:O42 C29:E38 N29:P38">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
update nhập hàng 7410 2in1 và 5310 i7
</commit_message>
<xml_diff>
--- a/BanLaptop/NhapXuatLaptop.xlsx
+++ b/BanLaptop/NhapXuatLaptop.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04.Private\BanLaptop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04D7403-FDEB-4BC1-B902-980FEB14009A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFBC37A-628E-438A-B5C3-6287FCE87E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="CTV" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NhapXuat!$K$1:$K$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NhapXuat!$K$1:$K$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="108">
   <si>
     <t>ID máy</t>
   </si>
@@ -330,6 +330,32 @@
   </si>
   <si>
     <t>Việt</t>
+  </si>
+  <si>
+    <t>9405508205497826574743</t>
+  </si>
+  <si>
+    <t>9405536104262700038858</t>
+  </si>
+  <si>
+    <t>9405508205497841021161</t>
+  </si>
+  <si>
+    <t>1Z11X45W0396452937</t>
+  </si>
+  <si>
+    <t>397108270831</t>
+  </si>
+  <si>
+    <t>Dell Latitude 7390 2-in-1 Laptop
+US $120.00</t>
+  </si>
+  <si>
+    <t>DELL Latitude 3410 i5-10210U 8 GB RAM 256 GB SSD FHD Backlit Keyboard!
+US $200.00</t>
+  </si>
+  <si>
+    <t>Dell Latitude 7400 2in1 (512GB SSD, Intel Core i7, 1.90GHz, 16GB) Laptop🔥US $246.50</t>
   </si>
 </sst>
 </file>
@@ -436,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -492,16 +518,10 @@
     <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -515,13 +535,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -813,34 +862,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q48"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N36" sqref="N36:N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.42578125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" style="25" customWidth="1"/>
     <col min="3" max="4" width="12.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="14" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="10.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.140625" style="3" customWidth="1"/>
     <col min="10" max="10" width="15.85546875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" style="20" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="27.28515625" style="20" customWidth="1"/>
     <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.42578125" style="10" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="33" t="s">
         <v>74</v>
       </c>
       <c r="B1" s="22" t="s">
@@ -893,7 +942,7 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="36">
+      <c r="A2" s="34">
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
@@ -937,7 +986,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="36">
+      <c r="A3" s="34">
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -949,7 +998,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7">
-        <f t="shared" ref="F3:F39" si="1">C3+D3+E3</f>
+        <f t="shared" ref="F3:F40" si="1">C3+D3+E3</f>
         <v>6500000</v>
       </c>
       <c r="G3" s="7">
@@ -981,7 +1030,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="36">
+      <c r="A4" s="34">
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
@@ -1025,7 +1074,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="36">
+      <c r="A5" s="34">
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
@@ -1071,7 +1120,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="36">
+      <c r="A6" s="34">
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
@@ -1113,7 +1162,7 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="36">
+      <c r="A7" s="34">
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
@@ -1157,7 +1206,7 @@
       <c r="Q7" s="6"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="36">
+      <c r="A8" s="34">
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
@@ -1201,7 +1250,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="36">
+      <c r="A9" s="34">
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
@@ -1245,7 +1294,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="36">
+      <c r="A10" s="34">
         <v>9</v>
       </c>
       <c r="B10" s="23" t="s">
@@ -1285,7 +1334,7 @@
       <c r="Q10" s="6"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="36">
+      <c r="A11" s="34">
         <v>10</v>
       </c>
       <c r="B11" s="23" t="s">
@@ -1329,7 +1378,7 @@
       <c r="Q11" s="6"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="36">
+      <c r="A12" s="34">
         <v>11</v>
       </c>
       <c r="B12" s="23" t="s">
@@ -1375,7 +1424,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="36">
+      <c r="A13" s="34">
         <v>12</v>
       </c>
       <c r="B13" s="23" t="s">
@@ -1419,7 +1468,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="36">
+      <c r="A14" s="34">
         <v>13</v>
       </c>
       <c r="B14" s="23" t="s">
@@ -1461,7 +1510,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="36">
+      <c r="A15" s="34">
         <v>14</v>
       </c>
       <c r="B15" s="23" t="s">
@@ -1505,7 +1554,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="36">
+      <c r="A16" s="34">
         <v>15</v>
       </c>
       <c r="B16" s="23" t="s">
@@ -1543,7 +1592,7 @@
       <c r="Q16" s="6"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="36">
+      <c r="A17" s="34">
         <v>16</v>
       </c>
       <c r="B17" s="23" t="s">
@@ -1583,7 +1632,7 @@
       <c r="Q17" s="6"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="36">
+      <c r="A18" s="34">
         <v>17</v>
       </c>
       <c r="B18" s="23" t="s">
@@ -1607,7 +1656,7 @@
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7">
-        <f t="shared" ref="J18:J44" si="4">H18-I18-F18</f>
+        <f t="shared" ref="J18:J48" si="4">H18-I18-F18</f>
         <v>500000</v>
       </c>
       <c r="K18" s="6" t="s">
@@ -1627,7 +1676,7 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="36">
+      <c r="A19" s="34">
         <v>18</v>
       </c>
       <c r="B19" s="23" t="s">
@@ -1669,7 +1718,7 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="36">
+      <c r="A20" s="34">
         <v>19</v>
       </c>
       <c r="B20" s="24" t="s">
@@ -1715,7 +1764,7 @@
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="36">
+      <c r="A21" s="34">
         <v>20</v>
       </c>
       <c r="B21" s="23" t="s">
@@ -1765,7 +1814,7 @@
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="36">
+      <c r="A22" s="34">
         <v>21</v>
       </c>
       <c r="B22" s="23" t="s">
@@ -1813,7 +1862,7 @@
       </c>
     </row>
     <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="36">
+      <c r="A23" s="34">
         <v>22</v>
       </c>
       <c r="B23" s="23" t="s">
@@ -1864,7 +1913,7 @@
       <c r="Q23" s="6"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="36">
+      <c r="A24" s="34">
         <v>23</v>
       </c>
       <c r="B24" s="23" t="s">
@@ -1910,7 +1959,7 @@
       <c r="Q24" s="6"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="36">
+      <c r="A25" s="34">
         <v>24</v>
       </c>
       <c r="B25" s="24" t="s">
@@ -1960,7 +2009,7 @@
       <c r="Q25" s="6"/>
     </row>
     <row r="26" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="36">
+      <c r="A26" s="34">
         <v>25</v>
       </c>
       <c r="B26" s="26" t="s">
@@ -2006,13 +2055,13 @@
       <c r="Q26" s="6"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" s="36">
+      <c r="A27" s="34">
         <v>26</v>
       </c>
       <c r="B27" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="31">
+      <c r="C27" s="40">
         <v>6537888</v>
       </c>
       <c r="D27" s="7">
@@ -2056,47 +2105,49 @@
       <c r="Q27" s="6"/>
     </row>
     <row r="28" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="36">
+      <c r="A28" s="34">
         <v>27</v>
       </c>
       <c r="B28" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="34">
+      <c r="C28" s="41">
         <v>7887859</v>
       </c>
-      <c r="D28" s="7"/>
+      <c r="D28" s="7">
+        <v>1000000</v>
+      </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7">
         <f t="shared" si="1"/>
-        <v>7887859</v>
+        <v>8887859</v>
       </c>
       <c r="G28" s="7">
         <f t="shared" si="6"/>
-        <v>9859823.75</v>
+        <v>11109823.75</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7">
         <f t="shared" si="4"/>
-        <v>-7887859</v>
+        <v>-8887859</v>
       </c>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
-      <c r="N28" s="32" t="s">
+      <c r="N28" s="31" t="s">
         <v>76</v>
       </c>
       <c r="O28" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="P28" s="33">
+      <c r="P28" s="32">
         <v>45016</v>
       </c>
       <c r="Q28" s="6"/>
     </row>
     <row r="29" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="36">
+      <c r="A29" s="34">
         <v>28</v>
       </c>
       <c r="B29" s="26" t="s">
@@ -2105,21 +2156,23 @@
       <c r="C29" s="7">
         <v>4850950</v>
       </c>
-      <c r="D29" s="7"/>
+      <c r="D29" s="7">
+        <v>1000000</v>
+      </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7">
         <f t="shared" si="1"/>
-        <v>4850950</v>
+        <v>5850950</v>
       </c>
       <c r="G29" s="7">
         <f t="shared" si="6"/>
-        <v>6063687.5</v>
+        <v>7313687.5</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7">
         <f t="shared" si="4"/>
-        <v>-4850950</v>
+        <v>-5850950</v>
       </c>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
@@ -2136,7 +2189,7 @@
       <c r="Q29" s="6"/>
     </row>
     <row r="30" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="36">
+      <c r="A30" s="34">
         <v>29</v>
       </c>
       <c r="B30" s="26" t="s">
@@ -2176,7 +2229,7 @@
       <c r="Q30" s="6"/>
     </row>
     <row r="31" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="36">
+      <c r="A31" s="34">
         <v>30</v>
       </c>
       <c r="B31" s="26" t="s">
@@ -2220,7 +2273,7 @@
       <c r="Q31" s="6"/>
     </row>
     <row r="32" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="36">
+      <c r="A32" s="34">
         <v>31</v>
       </c>
       <c r="B32" s="26" t="s">
@@ -2260,10 +2313,10 @@
       <c r="Q32" s="6"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A33" s="36">
+      <c r="A33" s="34">
         <v>32</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="35" t="s">
         <v>81</v>
       </c>
       <c r="C33" s="7">
@@ -2300,7 +2353,7 @@
       <c r="Q33" s="6"/>
     </row>
     <row r="34" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="36">
+      <c r="A34" s="34">
         <v>33</v>
       </c>
       <c r="B34" s="26" t="s">
@@ -2328,7 +2381,9 @@
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
-      <c r="N34" s="18"/>
+      <c r="N34" s="18" t="s">
+        <v>100</v>
+      </c>
       <c r="O34" s="6" t="s">
         <v>82</v>
       </c>
@@ -2338,7 +2393,7 @@
       <c r="Q34" s="6"/>
     </row>
     <row r="35" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="36">
+      <c r="A35" s="34">
         <v>34</v>
       </c>
       <c r="B35" s="26" t="s">
@@ -2378,7 +2433,7 @@
       <c r="Q35" s="6"/>
     </row>
     <row r="36" spans="1:17" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="36">
+      <c r="A36" s="34">
         <v>35</v>
       </c>
       <c r="B36" s="26" t="s">
@@ -2403,16 +2458,18 @@
       <c r="K36" s="6"/>
       <c r="L36" s="6"/>
       <c r="M36" s="6"/>
-      <c r="N36" s="18"/>
+      <c r="N36" s="18" t="s">
+        <v>101</v>
+      </c>
       <c r="O36" s="6"/>
       <c r="P36" s="8"/>
       <c r="Q36" s="6"/>
     </row>
     <row r="37" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="36">
+      <c r="A37" s="34">
         <v>36</v>
       </c>
-      <c r="B37" s="39" t="s">
+      <c r="B37" s="37" t="s">
         <v>94</v>
       </c>
       <c r="C37" s="7">
@@ -2434,122 +2491,222 @@
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
       <c r="M37" s="6"/>
-      <c r="N37" s="18"/>
+      <c r="N37" s="18" t="s">
+        <v>102</v>
+      </c>
       <c r="O37" s="6"/>
       <c r="P37" s="8"/>
       <c r="Q37" s="6"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="36">
+    <row r="38" spans="1:17" s="25" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="49">
         <v>37</v>
       </c>
-      <c r="B38" s="38"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7">
+      <c r="B38" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="50">
+        <v>3178000</v>
+      </c>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50">
+        <f t="shared" si="1"/>
+        <v>3178000</v>
+      </c>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="50">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="18"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="6"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A39" s="36">
+        <v>-3178000</v>
+      </c>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="O38" s="23"/>
+      <c r="P38" s="51"/>
+      <c r="Q38" s="23"/>
+    </row>
+    <row r="39" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="34">
         <v>38</v>
       </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="34"/>
+      <c r="B39" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="41">
+        <v>4560000</v>
+      </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4560000</v>
       </c>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
       <c r="J39" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-4560000</v>
       </c>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
-      <c r="N39" s="32"/>
+      <c r="N39" s="31" t="s">
+        <v>104</v>
+      </c>
       <c r="O39" s="6"/>
-      <c r="P39" s="33"/>
+      <c r="P39" s="32"/>
       <c r="Q39" s="6"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A40" s="36">
+    <row r="40" spans="1:17" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="34"/>
+      <c r="B40" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="7">
+        <v>6156000</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7">
+        <f t="shared" si="1"/>
+        <v>6156000</v>
+      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7">
+        <f t="shared" si="4"/>
+        <v>-6156000</v>
+      </c>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="6"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" s="34"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="6"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" s="34"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="44"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="45"/>
+      <c r="I42" s="45"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="46"/>
+      <c r="M42" s="46"/>
+      <c r="N42" s="47"/>
+      <c r="O42" s="46"/>
+      <c r="P42" s="48"/>
+      <c r="Q42" s="46"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" s="34"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
+      <c r="I43" s="45"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="46"/>
+      <c r="M43" s="46"/>
+      <c r="N43" s="47"/>
+      <c r="O43" s="46"/>
+      <c r="P43" s="48"/>
+      <c r="Q43" s="46"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" s="34">
         <v>39</v>
       </c>
-      <c r="C40" s="40"/>
-      <c r="J40" s="7"/>
-      <c r="N40" s="41"/>
-      <c r="P40" s="42"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A41" s="36">
+      <c r="C44" s="42"/>
+      <c r="J44" s="7"/>
+      <c r="N44" s="38"/>
+      <c r="P44" s="39"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="34">
         <v>40</v>
       </c>
-      <c r="C41" s="40"/>
-      <c r="J41" s="7"/>
-      <c r="N41" s="41"/>
-      <c r="P41" s="42"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A42" s="36"/>
-      <c r="C42" s="40"/>
-      <c r="J42" s="7"/>
-      <c r="N42" s="41"/>
-      <c r="P42" s="42"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J43" s="7">
+      <c r="C45" s="42"/>
+      <c r="J45" s="7"/>
+      <c r="N45" s="38"/>
+      <c r="P45" s="39"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="34"/>
+      <c r="C46" s="42"/>
+      <c r="J46" s="7"/>
+      <c r="N46" s="38"/>
+      <c r="P46" s="39"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J47" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C44" s="3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C48" s="3">
         <f>SUM(C2:C8)</f>
         <v>46150000</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H48" s="3">
         <f>SUM(H2:H8)</f>
         <v>50200000</v>
       </c>
-      <c r="J44" s="7">
+      <c r="J48" s="7">
         <f t="shared" si="4"/>
         <v>50200000</v>
       </c>
-      <c r="L44" t="s">
+      <c r="L48" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D48" s="3">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D52" s="3">
         <f>SUM(C20:C25)</f>
         <v>37301557</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="K1:K48" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="C2:F2 G2:M17 N2:P22 B2:B25 Q2:Q42 C3:E25 F3:F42 J3:J44 G18:I42 K18:M42 O23:P25 N26:P26 D26:E42 O26:O42 C29:E38 N29:P38">
+  <autoFilter ref="K1:K52" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="C2:F2 G2:M17 N2:P22 B2:B25 C3:E25 O23:P25 N26:P26 Q2:Q39 Q42:Q46 F3:F38 J3:J38 J42:J48 G18:I38 K18:M38 K42:M46 D26:E38 D39:M39 D42:I46 O26:O39 O42:O46 C29:E38 N29:P38 C40:Q41">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update máy mới về
</commit_message>
<xml_diff>
--- a/BanLaptop/NhapXuatLaptop.xlsx
+++ b/BanLaptop/NhapXuatLaptop.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\04.Private\BanLaptop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04.Private\BanLaptop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCEE751-0C48-4D0B-89B3-3293FB6D5589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3682D7-0827-4B14-A405-74AEFE9E71CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NhapXuat" sheetId="1" r:id="rId1"/>
@@ -24,23 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="129">
   <si>
     <t>ID máy</t>
   </si>
@@ -415,6 +404,21 @@
   </si>
   <si>
     <t>6tr</t>
+  </si>
+  <si>
+    <t>Chú Kiểm Nha Trang</t>
+  </si>
+  <si>
+    <t>397531124140</t>
+  </si>
+  <si>
+    <t>A Đoàn</t>
+  </si>
+  <si>
+    <t>Hiếu</t>
+  </si>
+  <si>
+    <t>6tr5</t>
   </si>
 </sst>
 </file>
@@ -1004,8 +1008,8 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,7 +1956,7 @@
         <v>45017</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
         <v>21</v>
       </c>
@@ -2000,7 +2004,7 @@
         <v>45016</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" s="44" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="38">
         <v>22</v>
       </c>
@@ -2051,7 +2055,7 @@
       </c>
       <c r="Q23" s="41"/>
     </row>
-    <row r="24" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="44" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="38">
         <v>23</v>
       </c>
@@ -2097,7 +2101,7 @@
       </c>
       <c r="Q24" s="41"/>
     </row>
-    <row r="25" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="44" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="38">
         <v>24</v>
       </c>
@@ -2147,7 +2151,7 @@
       </c>
       <c r="Q25" s="41"/>
     </row>
-    <row r="26" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" s="44" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="38">
         <v>25</v>
       </c>
@@ -2193,7 +2197,7 @@
       </c>
       <c r="Q26" s="41"/>
     </row>
-    <row r="27" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" s="44" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="38">
         <v>26</v>
       </c>
@@ -2330,7 +2334,7 @@
         <v>45019</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="56" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" s="56" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="66">
         <v>29</v>
       </c>
@@ -2360,6 +2364,9 @@
         <f t="shared" si="4"/>
         <v>-167935</v>
       </c>
+      <c r="K30" s="56" t="s">
+        <v>126</v>
+      </c>
       <c r="N30" s="57" t="s">
         <v>85</v>
       </c>
@@ -2477,11 +2484,13 @@
         <f t="shared" si="6"/>
         <v>6948677.5</v>
       </c>
-      <c r="H33" s="7"/>
+      <c r="H33" s="7" t="s">
+        <v>122</v>
+      </c>
       <c r="I33" s="7"/>
-      <c r="J33" s="7">
+      <c r="J33" s="7" t="e">
         <f t="shared" si="4"/>
-        <v>-5558942</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N33" s="18" t="s">
         <v>83</v>
@@ -2678,8 +2687,8 @@
       </c>
       <c r="P38" s="37"/>
     </row>
-    <row r="39" spans="1:16" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="67">
+    <row r="39" spans="1:16" s="6" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="70">
         <v>38</v>
       </c>
       <c r="B39" s="22" t="s">
@@ -2700,21 +2709,28 @@
         <f t="shared" si="6"/>
         <v>6762500</v>
       </c>
-      <c r="H39" s="7" t="s">
-        <v>122</v>
+      <c r="H39" s="7">
+        <v>7000000</v>
       </c>
       <c r="I39" s="7"/>
-      <c r="J39" s="7" t="e">
+      <c r="J39" s="7">
         <f t="shared" si="4"/>
-        <v>#VALUE!</v>
+        <v>1590000</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="N39" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="P39" s="27"/>
+      <c r="P39" s="27">
+        <v>45265</v>
+      </c>
     </row>
     <row r="40" spans="1:16" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="67"/>
+      <c r="A40" s="70">
+        <v>39</v>
+      </c>
       <c r="B40" s="71" t="s">
         <v>107</v>
       </c>
@@ -2747,7 +2763,9 @@
       <c r="P40" s="8"/>
     </row>
     <row r="41" spans="1:16" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="67"/>
+      <c r="A41" s="70">
+        <v>40</v>
+      </c>
       <c r="B41" s="71" t="s">
         <v>108</v>
       </c>
@@ -2766,11 +2784,13 @@
         <f t="shared" si="6"/>
         <v>6220000</v>
       </c>
-      <c r="H41" s="7"/>
+      <c r="H41" s="7" t="s">
+        <v>122</v>
+      </c>
       <c r="I41" s="7"/>
-      <c r="J41" s="7">
+      <c r="J41" s="7" t="e">
         <f t="shared" si="4"/>
-        <v>-4976000</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N41" s="18" t="s">
         <v>109</v>
@@ -2778,34 +2798,44 @@
       <c r="P41" s="8"/>
     </row>
     <row r="42" spans="1:16" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="67"/>
+      <c r="A42" s="70">
+        <v>41</v>
+      </c>
       <c r="B42" s="22" t="s">
         <v>111</v>
       </c>
       <c r="C42" s="34">
         <v>3192000</v>
       </c>
-      <c r="D42" s="7"/>
+      <c r="D42" s="36">
+        <v>850000</v>
+      </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7">
         <f t="shared" si="1"/>
-        <v>3192000</v>
+        <v>4042000</v>
       </c>
       <c r="G42" s="7">
         <f t="shared" si="6"/>
-        <v>3990000</v>
-      </c>
-      <c r="H42" s="7"/>
+        <v>5052500</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>128</v>
+      </c>
       <c r="I42" s="7"/>
-      <c r="J42" s="7">
+      <c r="J42" s="7" t="e">
         <f t="shared" si="4"/>
-        <v>-3192000</v>
-      </c>
-      <c r="N42" s="26"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N42" s="26" t="s">
+        <v>125</v>
+      </c>
       <c r="P42" s="27"/>
     </row>
-    <row r="43" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="67"/>
+    <row r="43" spans="1:16" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="70">
+        <v>42</v>
+      </c>
       <c r="B43" s="69" t="s">
         <v>112</v>
       </c>
@@ -2824,11 +2854,16 @@
         <f t="shared" si="6"/>
         <v>8643750</v>
       </c>
-      <c r="H43" s="7"/>
+      <c r="H43" s="7">
+        <v>8500000</v>
+      </c>
       <c r="I43" s="7"/>
       <c r="J43" s="7">
         <f t="shared" si="4"/>
-        <v>-6915000</v>
+        <v>1585000</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>124</v>
       </c>
       <c r="N43" s="26" t="s">
         <v>113</v>
@@ -2836,8 +2871,8 @@
       <c r="P43" s="27"/>
     </row>
     <row r="44" spans="1:16" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="67">
-        <v>39</v>
+      <c r="A44" s="70">
+        <v>43</v>
       </c>
       <c r="B44" s="31" t="s">
         <v>120</v>
@@ -2845,21 +2880,25 @@
       <c r="C44" s="34">
         <v>3268000</v>
       </c>
-      <c r="D44" s="7"/>
+      <c r="D44" s="7">
+        <v>850000</v>
+      </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7">
         <f t="shared" si="1"/>
-        <v>3268000</v>
+        <v>4118000</v>
       </c>
       <c r="G44" s="7">
         <f t="shared" si="6"/>
-        <v>4085000</v>
-      </c>
-      <c r="H44" s="7"/>
+        <v>5147500</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>122</v>
+      </c>
       <c r="I44" s="7"/>
-      <c r="J44" s="7">
+      <c r="J44" s="7" t="e">
         <f t="shared" si="4"/>
-        <v>-3268000</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N44" s="73" t="s">
         <v>121</v>
@@ -2913,7 +2952,7 @@
     </row>
   </sheetData>
   <autoFilter ref="K1:K52" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="C2:F2 G2:M17 N2:P22 B2:B25 C3:E25 O23:P25 N26:P26 Q2:Q39 F3:F38 J3:J38 G18:I35 K18:M38 K42:M46 D26:E38 O26:O39 C29:E38 N29:P38 H40:Q41 D42:F42 H42:I42 H39:M39 H36:I38 G36:G42 D39:F39 C40:F41 Q42:Q43 Q45:Q46 P44 O42:O43 O45:O46 D43:I46 J42:J48">
+  <conditionalFormatting sqref="C2:F2 G2:M17 N2:P22 B2:B25 Q2:Q39 C3:E25 F3:F38 J3:J38 G18:I35 K18:M38 O23:P25 N26:P26 D26:E38 O26:O39 C29:E38 N29:P38 H36:I38 G36:G42 D39:F39 H39:M39 C40:F41 H40:Q41 H42:I42 O42:O43 Q42:Q43 K42:M46 J42:J48 P44 O45:O46 Q45:Q46 D42:F42 D43:I46">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Keep nhap xuat only
</commit_message>
<xml_diff>
--- a/BanLaptop/NhapXuatLaptop.xlsx
+++ b/BanLaptop/NhapXuatLaptop.xlsx
@@ -1,35 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04.Private\BanLaptop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\04.Private\BanLaptop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66191150-EFA4-4D27-BFD2-EC3895D56A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8A8C6C1-C72F-4D27-98F7-071F36FB7B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NhapXuat" sheetId="1" r:id="rId1"/>
     <sheet name="CTV" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NhapXuat!$K$1:$K$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NhapXuat!$L$1:$L$52</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="148">
   <si>
     <t>ID máy</t>
   </si>
@@ -422,6 +433,60 @@
   </si>
   <si>
     <t>17/05/23</t>
+  </si>
+  <si>
+    <t>Giá CTV</t>
+  </si>
+  <si>
+    <t>Dell Latitude 7390 2-in-1 Laptop</t>
+  </si>
+  <si>
+    <t>A Minh béo</t>
+  </si>
+  <si>
+    <t>10tr5</t>
+  </si>
+  <si>
+    <t>13tr5</t>
+  </si>
+  <si>
+    <t>Dell Inspiron 13 5310 13.3" (512GB SSD, Intel Core i5-11320H, 2.50GHz, 16GB RAM) Like new</t>
+  </si>
+  <si>
+    <t>Dell Inspiron 13 5310 13.3 " Core i5-11320H/16GB/512GB SSD  Cấn nhẹ mặt trên, mất nhựa che camera</t>
+  </si>
+  <si>
+    <t>Dell Latitude 7400 2in1 (512GB SSD, Intel Core i7, 1.90GHz, 16GB) Máy đẹp</t>
+  </si>
+  <si>
+    <t>Dell Latitude 7400 14" Intel i5-8265U@1.60GHz 8GB RAM 256GB SSD WiFi HDMI Win11US Xước đít</t>
+  </si>
+  <si>
+    <t>Dell Latitude 5400 14" (256GB SSD, Intel Core i5-8265u 1.6GHz, 8GB) máy đẹp</t>
+  </si>
+  <si>
+    <t>Dell Latitude 5400 Laptop: Work, School (256 GB SSD, Intel Core i5, 16GB RAM)  Máy đẹp</t>
+  </si>
+  <si>
+    <t>Giá bán ctv Công thức</t>
+  </si>
+  <si>
+    <t>9tr</t>
+  </si>
+  <si>
+    <t>5tr</t>
+  </si>
+  <si>
+    <t>10tr-10tr5</t>
+  </si>
+  <si>
+    <t>11tr5</t>
+  </si>
+  <si>
+    <t>8tr5</t>
+  </si>
+  <si>
+    <t>5tr5</t>
   </si>
 </sst>
 </file>
@@ -432,7 +497,7 @@
     <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,6 +525,20 @@
       <color rgb="FF191919"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -512,7 +591,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -559,18 +638,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -719,12 +808,41 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1008,1966 +1126,2066 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="74.140625" style="24" customWidth="1"/>
-    <col min="3" max="4" width="12.140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.28515625" style="20" customWidth="1"/>
-    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="74.140625" style="21" customWidth="1"/>
+    <col min="3" max="4" width="12.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="2" customWidth="1"/>
+    <col min="6" max="7" width="10.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.28515625" style="17" customWidth="1"/>
+    <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="L1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="O1" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="Q1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="R1" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29">
+    <row r="2" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="4">
         <v>6700000</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4">
         <f>C2+D2+E2</f>
         <v>6700000</v>
       </c>
-      <c r="G2" s="7">
-        <f t="shared" ref="G2:G17" si="0">(F2*25%)+F2</f>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4">
+        <f t="shared" ref="H2:H17" si="0">(F2*25%)+F2</f>
         <v>8375000</v>
       </c>
-      <c r="H2" s="7">
+      <c r="I2" s="4">
         <v>7600000</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7">
-        <f>H2-I2-F2</f>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4">
+        <f>I2-J2-F2</f>
         <v>900000</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6">
+      <c r="M2" s="3"/>
+      <c r="N2" s="3">
         <v>34534861886</v>
       </c>
-      <c r="N2" s="18"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="8">
+      <c r="O2" s="15"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="5">
         <v>44835</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="R2" s="6">
         <v>44835</v>
       </c>
     </row>
-    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29">
+    <row r="3" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="4">
         <v>6500000</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4">
         <f t="shared" ref="F3:F44" si="1">C3+D3+E3</f>
         <v>6500000</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4">
         <f t="shared" si="0"/>
         <v>8125000</v>
       </c>
-      <c r="H3" s="7">
+      <c r="I3" s="4">
         <v>7250000</v>
       </c>
-      <c r="I3" s="7">
+      <c r="J3" s="4">
         <v>5000</v>
       </c>
-      <c r="J3" s="7">
-        <f t="shared" ref="J3:J17" si="2">H3-I3-F3</f>
+      <c r="K3" s="4">
+        <f t="shared" ref="K3:K17" si="2">I3-J3-F3</f>
         <v>745000</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="18"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="8">
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="5">
         <v>44835</v>
       </c>
-      <c r="Q3" s="9">
+      <c r="R3" s="6">
         <v>44835</v>
       </c>
     </row>
-    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29">
+    <row r="4" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
         <v>3</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="4">
         <v>4900000</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4">
         <f t="shared" si="1"/>
         <v>4900000</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4">
         <f t="shared" si="0"/>
         <v>6125000</v>
       </c>
-      <c r="H4" s="7">
+      <c r="I4" s="4">
         <v>5400000</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7">
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
         <f t="shared" si="2"/>
         <v>500000</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="3"/>
+      <c r="N4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N4" s="18"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="8">
+      <c r="O4" s="15"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="5">
         <v>44841</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="R4" s="6">
         <v>44814</v>
       </c>
     </row>
-    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29">
+    <row r="5" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
         <v>4</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="4">
         <v>6700000</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4">
         <f t="shared" si="1"/>
         <v>6700000</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4">
         <f t="shared" si="0"/>
         <v>8375000</v>
       </c>
-      <c r="H5" s="7">
+      <c r="I5" s="4">
         <v>7600000</v>
       </c>
-      <c r="I5" s="7">
+      <c r="J5" s="4">
         <v>420000</v>
       </c>
-      <c r="J5" s="7">
+      <c r="K5" s="4">
         <f t="shared" si="2"/>
         <v>480000</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="L5" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="3"/>
+      <c r="N5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="18"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="8">
+      <c r="O5" s="15"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="5">
         <v>44841</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="R5" s="6">
         <v>44841</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="29">
+    <row r="6" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26">
         <v>5</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="4">
         <v>7150000</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4">
         <f t="shared" si="1"/>
         <v>7150000</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4">
         <f t="shared" si="0"/>
         <v>8937500</v>
       </c>
-      <c r="H6" s="7">
+      <c r="I6" s="4">
         <v>7500000</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7">
+      <c r="J6" s="4"/>
+      <c r="K6" s="4">
         <f t="shared" si="2"/>
         <v>350000</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="L6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="3"/>
+      <c r="N6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N6" s="18"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="8">
+      <c r="O6" s="15"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="5">
         <v>44842</v>
       </c>
-      <c r="Q6" s="6"/>
-    </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29">
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26">
         <v>6</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="4">
         <v>7500000</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4">
         <f t="shared" si="1"/>
         <v>7500000</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="4"/>
+      <c r="H7" s="4">
         <f t="shared" si="0"/>
         <v>9375000</v>
       </c>
-      <c r="H7" s="7">
+      <c r="I7" s="4">
         <v>7500000</v>
       </c>
-      <c r="I7" s="7">
+      <c r="J7" s="4">
         <v>10000</v>
       </c>
-      <c r="J7" s="7">
+      <c r="K7" s="4">
         <f t="shared" si="2"/>
         <v>-10000</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="L7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6" t="s">
+      <c r="M7" s="3"/>
+      <c r="N7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="N7" s="18"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="8">
+      <c r="O7" s="15"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="5">
         <v>44845</v>
       </c>
-      <c r="Q7" s="6"/>
-    </row>
-    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
+      <c r="R7" s="3"/>
+    </row>
+    <row r="8" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26">
         <v>7</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="4">
         <v>6700000</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4">
         <f t="shared" si="1"/>
         <v>6700000</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="4"/>
+      <c r="H8" s="4">
         <f t="shared" si="0"/>
         <v>8375000</v>
       </c>
-      <c r="H8" s="7">
+      <c r="I8" s="4">
         <v>7350000</v>
       </c>
-      <c r="I8" s="7">
+      <c r="J8" s="4">
         <v>10000</v>
       </c>
-      <c r="J8" s="7">
+      <c r="K8" s="4">
         <f t="shared" si="2"/>
         <v>640000</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="L8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="8">
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="5">
         <v>44841</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="R8" s="6">
         <v>44841</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29">
+    <row r="9" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="26">
         <v>8</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="4">
         <v>11500000</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4">
         <f t="shared" si="1"/>
         <v>11500000</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4">
         <f t="shared" si="0"/>
         <v>14375000</v>
       </c>
-      <c r="H9" s="7">
+      <c r="I9" s="4">
         <v>12000000</v>
       </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7">
+      <c r="J9" s="4"/>
+      <c r="K9" s="4">
         <f t="shared" si="2"/>
         <v>500000</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="L9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6" t="s">
+      <c r="M9" s="3"/>
+      <c r="N9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="8">
+      <c r="O9" s="15"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="5">
         <v>44876</v>
       </c>
-      <c r="Q9" s="6" t="s">
+      <c r="R9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29">
+    <row r="10" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="26">
         <v>9</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="4">
         <v>6500000</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4">
         <f t="shared" si="1"/>
         <v>6500000</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="4"/>
+      <c r="H10" s="4">
         <f t="shared" si="0"/>
         <v>8125000</v>
       </c>
-      <c r="H10" s="7">
+      <c r="I10" s="4">
         <v>7500000</v>
       </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7">
+      <c r="J10" s="4"/>
+      <c r="K10" s="4">
         <f t="shared" si="2"/>
         <v>1000000</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="L10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="8">
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="5">
         <v>44883</v>
       </c>
-      <c r="Q10" s="6"/>
-    </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29">
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26">
         <v>10</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="4">
         <v>6500000</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4">
         <f t="shared" si="1"/>
         <v>6500000</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="4"/>
+      <c r="H11" s="4">
         <f t="shared" si="0"/>
         <v>8125000</v>
       </c>
-      <c r="H11" s="7">
+      <c r="I11" s="4">
         <v>6900000</v>
       </c>
-      <c r="I11" s="7">
+      <c r="J11" s="4">
         <v>100000</v>
       </c>
-      <c r="J11" s="7">
+      <c r="K11" s="4">
         <f t="shared" si="2"/>
         <v>300000</v>
       </c>
-      <c r="K11" s="6" t="s">
+      <c r="L11" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6" t="s">
+      <c r="M11" s="3"/>
+      <c r="N11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N11" s="18"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="8">
+      <c r="O11" s="15"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="5">
         <v>44883</v>
       </c>
-      <c r="Q11" s="6"/>
-    </row>
-    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29">
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26">
         <v>11</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="4">
         <v>5000000</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4">
         <f t="shared" si="1"/>
         <v>5000000</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4">
         <f t="shared" si="0"/>
         <v>6250000</v>
       </c>
-      <c r="H12" s="7">
+      <c r="I12" s="4">
         <v>5800000</v>
       </c>
-      <c r="I12" s="7">
+      <c r="J12" s="4">
         <v>5000</v>
       </c>
-      <c r="J12" s="7">
+      <c r="K12" s="4">
         <f t="shared" si="2"/>
         <v>795000</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="L12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="M12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M12" s="6"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="8">
+      <c r="N12" s="3"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="5">
         <v>44896</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="R12" s="6">
         <v>44841</v>
       </c>
     </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
+    <row r="13" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26">
         <v>12</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="4">
         <v>5500000</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4">
         <f t="shared" si="1"/>
         <v>5500000</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="4"/>
+      <c r="H13" s="4">
         <f t="shared" si="0"/>
         <v>6875000</v>
       </c>
-      <c r="H13" s="7">
+      <c r="I13" s="4">
         <v>6300000</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7">
+      <c r="J13" s="4"/>
+      <c r="K13" s="4">
         <f t="shared" si="2"/>
         <v>800000</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="L13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="M13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="8">
+      <c r="N13" s="3"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="5">
         <v>44937</v>
       </c>
-      <c r="Q13" s="8">
+      <c r="R13" s="5">
         <v>44938</v>
       </c>
     </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29">
+    <row r="14" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26">
         <v>13</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="4">
         <v>5500000</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4">
         <f t="shared" si="1"/>
         <v>5500000</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4">
         <f t="shared" si="0"/>
         <v>6875000</v>
       </c>
-      <c r="H14" s="7">
+      <c r="I14" s="4">
         <v>6600000</v>
       </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7">
+      <c r="J14" s="4"/>
+      <c r="K14" s="4">
         <f t="shared" si="2"/>
         <v>1100000</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="L14" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="8">
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="5">
         <v>44938</v>
       </c>
-      <c r="Q14" s="8">
+      <c r="R14" s="5">
         <v>44939</v>
       </c>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29">
+    <row r="15" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
         <v>14</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="4">
         <v>5700000</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4">
         <f t="shared" si="1"/>
         <v>5700000</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="4"/>
+      <c r="H15" s="4">
         <f t="shared" si="0"/>
         <v>7125000</v>
       </c>
-      <c r="H15" s="7">
+      <c r="I15" s="4">
         <v>6200000</v>
       </c>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7">
+      <c r="J15" s="4"/>
+      <c r="K15" s="4">
         <f t="shared" si="2"/>
         <v>500000</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="L15" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="M15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M15" s="6"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="8">
+      <c r="N15" s="3"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="5">
         <v>44957</v>
       </c>
-      <c r="Q15" s="8">
+      <c r="R15" s="5">
         <v>44957</v>
       </c>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29">
+    <row r="16" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26">
         <v>15</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="4">
         <v>8000000</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
         <v>8000000</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="4"/>
+      <c r="H16" s="4">
         <f t="shared" si="0"/>
         <v>10000000</v>
       </c>
-      <c r="H16" s="7">
+      <c r="I16" s="4">
         <v>10500000</v>
       </c>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7">
+      <c r="J16" s="4"/>
+      <c r="K16" s="4">
         <f t="shared" si="2"/>
         <v>2500000</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="L16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="6"/>
-    </row>
-    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29">
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="26">
         <v>16</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="4">
         <v>9693017</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="4">
         <v>1142570</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4">
         <f t="shared" si="1"/>
         <v>10835587</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="4"/>
+      <c r="H17" s="4">
         <f t="shared" si="0"/>
         <v>13544483.75</v>
       </c>
-      <c r="H17" s="7">
+      <c r="I17" s="4">
         <v>14000000</v>
       </c>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7">
+      <c r="J17" s="4"/>
+      <c r="K17" s="4">
         <f t="shared" si="2"/>
         <v>3164413</v>
       </c>
-      <c r="K17" s="6" t="s">
+      <c r="L17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="18"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="6"/>
-    </row>
-    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="3"/>
+    </row>
+    <row r="18" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26">
         <v>17</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="4">
         <v>5000000</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4">
         <f t="shared" si="1"/>
         <v>5000000</v>
       </c>
-      <c r="G18" s="7">
-        <f t="shared" ref="G18" si="3">(F18*25%)+F18</f>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4">
+        <f t="shared" ref="H18" si="3">(F18*25%)+F18</f>
         <v>6250000</v>
       </c>
-      <c r="H18" s="7">
+      <c r="I18" s="4">
         <v>5500000</v>
       </c>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7">
-        <f t="shared" ref="J18:J48" si="4">H18-I18-F18</f>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4">
+        <f t="shared" ref="K18:K48" si="4">I18-J18-F18</f>
         <v>500000</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="L18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L18" s="6" t="s">
+      <c r="M18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M18" s="6" t="s">
+      <c r="N18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="N18" s="18"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="6" t="s">
+      <c r="O18" s="15"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
+    <row r="19" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26">
         <v>18</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="4">
         <v>4500000</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7">
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4">
         <f t="shared" si="1"/>
         <v>4500000</v>
       </c>
-      <c r="G19" s="7">
-        <f t="shared" ref="G19" si="5">(F19*25%)+F19</f>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4">
+        <f t="shared" ref="H19" si="5">(F19*25%)+F19</f>
         <v>5625000</v>
       </c>
-      <c r="H19" s="7">
+      <c r="I19" s="4">
         <v>5500000</v>
       </c>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7">
+      <c r="J19" s="4"/>
+      <c r="K19" s="4">
         <f t="shared" si="4"/>
         <v>1000000</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="L19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L19" s="6" t="s">
+      <c r="M19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M19" s="6"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="6" t="s">
+      <c r="N19" s="3"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29">
+    <row r="20" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26">
         <v>19</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="16">
+      <c r="C20" s="13">
         <v>6794437</v>
       </c>
-      <c r="D20" s="16">
+      <c r="D20" s="13">
         <v>1189453</v>
       </c>
-      <c r="E20" s="16"/>
-      <c r="F20" s="7">
+      <c r="E20" s="13"/>
+      <c r="F20" s="4">
         <f t="shared" si="1"/>
         <v>7983890</v>
       </c>
-      <c r="G20" s="16">
-        <f t="shared" ref="G20:G44" si="6">(F20*25%)+F20</f>
+      <c r="G20" s="4"/>
+      <c r="H20" s="13">
+        <f t="shared" ref="H20:H44" si="6">(F20*25%)+F20</f>
         <v>9979862.5</v>
       </c>
-      <c r="H20" s="16">
+      <c r="I20" s="13">
         <v>9500000</v>
       </c>
-      <c r="I20" s="16">
+      <c r="J20" s="13">
         <v>50000</v>
       </c>
-      <c r="J20" s="7">
+      <c r="K20" s="4">
         <f t="shared" si="4"/>
         <v>1466110</v>
       </c>
-      <c r="K20" s="6" t="s">
+      <c r="L20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14" t="s">
+      <c r="M20" s="11"/>
+      <c r="N20" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="N20" s="19"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="8">
+      <c r="O20" s="16"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="5">
         <v>45019</v>
       </c>
     </row>
-    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29">
+    <row r="21" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="26">
         <v>20</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="4">
         <v>7839722</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="4">
         <v>1109083</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="4">
         <v>300000</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="4">
         <f t="shared" si="1"/>
         <v>9248805</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="4"/>
+      <c r="H21" s="4">
         <f t="shared" si="6"/>
         <v>11561006.25</v>
       </c>
-      <c r="H21" s="7">
+      <c r="I21" s="4">
         <v>12000000</v>
       </c>
-      <c r="I21" s="7">
+      <c r="J21" s="4">
         <v>1500000</v>
       </c>
-      <c r="J21" s="7">
+      <c r="K21" s="4">
         <f t="shared" si="4"/>
         <v>1251195</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="L21" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6" t="s">
+      <c r="M21" s="3"/>
+      <c r="N21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="N21" s="18"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="8">
+      <c r="O21" s="15"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="5">
         <v>45049</v>
       </c>
-      <c r="Q21" s="8">
+      <c r="R21" s="5">
         <v>45017</v>
       </c>
     </row>
-    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="29">
+    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="26">
         <v>21</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="4">
         <v>9561005</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="4">
         <v>1000000</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4">
         <f t="shared" si="1"/>
         <v>10561005</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="4"/>
+      <c r="H22" s="4">
         <f t="shared" si="6"/>
         <v>13201256.25</v>
       </c>
-      <c r="H22" s="7">
+      <c r="I22" s="4">
         <v>12000000</v>
       </c>
-      <c r="I22" s="7">
+      <c r="J22" s="4">
         <v>900000</v>
       </c>
-      <c r="J22" s="7">
+      <c r="K22" s="4">
         <f t="shared" si="4"/>
         <v>538995</v>
       </c>
-      <c r="K22" s="6" t="s">
+      <c r="L22" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="6" t="s">
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P22" s="8" t="s">
+      <c r="Q22" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="Q22" s="8">
+      <c r="R22" s="5">
         <v>45016</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="44" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38">
+    <row r="23" spans="1:18" s="41" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="35">
         <v>22</v>
       </c>
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="40">
+      <c r="C23" s="37">
         <f>5182073+150000</f>
         <v>5332073</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="37">
         <v>1375000</v>
       </c>
-      <c r="E23" s="40">
+      <c r="E23" s="37">
         <v>-1000000</v>
       </c>
-      <c r="F23" s="40">
+      <c r="F23" s="37">
         <f>C23+D23+E23</f>
         <v>5707073</v>
       </c>
-      <c r="G23" s="40">
+      <c r="G23" s="37"/>
+      <c r="H23" s="37">
         <f>(F23*25%)+F23</f>
         <v>7133841.25</v>
       </c>
-      <c r="H23" s="40">
+      <c r="I23" s="37">
         <v>8200000</v>
       </c>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40">
+      <c r="J23" s="37"/>
+      <c r="K23" s="37">
         <f t="shared" si="4"/>
         <v>2492927</v>
       </c>
-      <c r="K23" s="41" t="s">
+      <c r="L23" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41" t="s">
+      <c r="M23" s="38"/>
+      <c r="N23" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="N23" s="46" t="s">
+      <c r="O23" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="O23" s="41" t="s">
+      <c r="P23" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P23" s="43">
+      <c r="Q23" s="40">
         <v>45010</v>
       </c>
-      <c r="Q23" s="41"/>
-    </row>
-    <row r="24" spans="1:17" s="44" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38">
+      <c r="R23" s="38"/>
+    </row>
+    <row r="24" spans="1:18" s="41" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="35">
         <v>23</v>
       </c>
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="40">
+      <c r="C24" s="37">
         <v>3281172</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="37">
         <v>1075000</v>
       </c>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40">
+      <c r="E24" s="37"/>
+      <c r="F24" s="37">
         <f t="shared" si="1"/>
         <v>4356172</v>
       </c>
-      <c r="G24" s="40">
+      <c r="G24" s="37"/>
+      <c r="H24" s="37">
         <f t="shared" si="6"/>
         <v>5445215</v>
       </c>
-      <c r="H24" s="40">
+      <c r="I24" s="37">
         <v>6400000</v>
       </c>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40">
+      <c r="J24" s="37"/>
+      <c r="K24" s="37">
         <f t="shared" si="4"/>
         <v>2043828</v>
       </c>
-      <c r="K24" s="41" t="s">
+      <c r="L24" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="46" t="s">
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="O24" s="41" t="s">
+      <c r="P24" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P24" s="43">
+      <c r="Q24" s="40">
         <v>45011</v>
       </c>
-      <c r="Q24" s="41"/>
-    </row>
-    <row r="25" spans="1:17" s="44" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38">
+      <c r="R24" s="38"/>
+    </row>
+    <row r="25" spans="1:18" s="41" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="35">
         <v>24</v>
       </c>
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="40">
+      <c r="C25" s="37">
         <v>4493148</v>
       </c>
-      <c r="D25" s="40">
+      <c r="D25" s="37">
         <v>1075000</v>
       </c>
-      <c r="E25" s="40">
+      <c r="E25" s="37">
         <v>490000</v>
       </c>
-      <c r="F25" s="40">
+      <c r="F25" s="37">
         <f t="shared" si="1"/>
         <v>6058148</v>
       </c>
-      <c r="G25" s="40">
+      <c r="G25" s="37"/>
+      <c r="H25" s="37">
         <f t="shared" si="6"/>
         <v>7572685</v>
       </c>
-      <c r="H25" s="40">
+      <c r="I25" s="37">
         <v>8000000</v>
       </c>
-      <c r="I25" s="40"/>
-      <c r="J25" s="40">
+      <c r="J25" s="37"/>
+      <c r="K25" s="37">
         <f t="shared" si="4"/>
         <v>1941852</v>
       </c>
-      <c r="K25" s="41" t="s">
+      <c r="L25" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41" t="s">
+      <c r="M25" s="38"/>
+      <c r="N25" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="N25" s="46" t="s">
+      <c r="O25" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="O25" s="41" t="s">
+      <c r="P25" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P25" s="43">
+      <c r="Q25" s="40">
         <v>45012</v>
       </c>
-      <c r="Q25" s="41"/>
-    </row>
-    <row r="26" spans="1:17" s="44" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="38">
+      <c r="R25" s="38"/>
+    </row>
+    <row r="26" spans="1:18" s="41" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="35">
         <v>25</v>
       </c>
-      <c r="B26" s="39" t="s">
+      <c r="B26" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="47">
+      <c r="C26" s="44">
         <v>3801801</v>
       </c>
-      <c r="D26" s="40">
+      <c r="D26" s="37">
         <v>1075000</v>
       </c>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40">
+      <c r="E26" s="37"/>
+      <c r="F26" s="37">
         <f t="shared" si="1"/>
         <v>4876801</v>
       </c>
-      <c r="G26" s="40">
+      <c r="G26" s="37"/>
+      <c r="H26" s="37">
         <f t="shared" si="6"/>
         <v>6096001.25</v>
       </c>
-      <c r="H26" s="40">
+      <c r="I26" s="37">
         <v>7950000</v>
       </c>
-      <c r="I26" s="40"/>
-      <c r="J26" s="40">
+      <c r="J26" s="37"/>
+      <c r="K26" s="37">
         <f t="shared" si="4"/>
         <v>3073199</v>
       </c>
-      <c r="K26" s="41" t="s">
+      <c r="L26" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="42" t="s">
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="O26" s="41" t="s">
+      <c r="P26" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P26" s="43">
+      <c r="Q26" s="40">
         <v>45017</v>
       </c>
-      <c r="Q26" s="41"/>
-    </row>
-    <row r="27" spans="1:17" s="44" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="38">
+      <c r="R26" s="38"/>
+    </row>
+    <row r="27" spans="1:18" s="41" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="35">
         <v>26</v>
       </c>
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="60">
+      <c r="C27" s="57">
         <v>6537888</v>
       </c>
-      <c r="D27" s="61">
+      <c r="D27" s="58">
         <v>1050000</v>
       </c>
-      <c r="E27" s="61">
+      <c r="E27" s="58">
         <v>200000</v>
       </c>
-      <c r="F27" s="61">
+      <c r="F27" s="58">
         <f t="shared" si="1"/>
         <v>7787888</v>
       </c>
-      <c r="G27" s="61">
+      <c r="G27" s="58"/>
+      <c r="H27" s="58">
         <f t="shared" si="6"/>
         <v>9734860</v>
       </c>
-      <c r="H27" s="61">
+      <c r="I27" s="58">
         <v>9500000</v>
       </c>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61">
+      <c r="J27" s="58"/>
+      <c r="K27" s="58">
         <f t="shared" si="4"/>
         <v>1712112</v>
       </c>
-      <c r="K27" s="62" t="s">
+      <c r="L27" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62" t="s">
+      <c r="M27" s="59"/>
+      <c r="N27" s="59" t="s">
         <v>91</v>
       </c>
-      <c r="N27" s="63" t="s">
+      <c r="O27" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="O27" s="62" t="s">
+      <c r="P27" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="P27" s="64">
+      <c r="Q27" s="61">
         <v>45015</v>
       </c>
-      <c r="Q27" s="62"/>
-    </row>
-    <row r="28" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="65">
+      <c r="R27" s="59"/>
+    </row>
+    <row r="28" spans="1:18" s="38" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="62">
         <v>27</v>
       </c>
-      <c r="B28" s="48" t="s">
+      <c r="B28" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="49">
+      <c r="C28" s="46">
         <v>7887859</v>
       </c>
-      <c r="D28" s="50">
+      <c r="D28" s="47">
         <v>1800000</v>
       </c>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50">
+      <c r="E28" s="47"/>
+      <c r="F28" s="47">
         <f t="shared" si="1"/>
         <v>9687859</v>
       </c>
-      <c r="G28" s="50">
+      <c r="G28" s="47">
+        <f>(F28*15%)+F28</f>
+        <v>11141037.85</v>
+      </c>
+      <c r="H28" s="47">
         <f t="shared" si="6"/>
         <v>12109823.75</v>
       </c>
-      <c r="H28" s="50">
+      <c r="I28" s="47">
         <v>16700000</v>
       </c>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50">
+      <c r="J28" s="47"/>
+      <c r="K28" s="47">
         <f t="shared" si="4"/>
         <v>7012141</v>
       </c>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51" t="s">
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
+      <c r="N28" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="N28" s="52" t="s">
+      <c r="O28" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="O28" s="51" t="s">
+      <c r="P28" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="P28" s="53">
+      <c r="Q28" s="50">
         <v>45016</v>
       </c>
-      <c r="Q28" s="51" t="s">
+      <c r="R28" s="48" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="41" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="65">
+    <row r="29" spans="1:18" s="38" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="62">
         <v>28</v>
       </c>
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="40">
+      <c r="C29" s="37">
         <v>4850950</v>
       </c>
-      <c r="D29" s="40">
+      <c r="D29" s="37">
         <v>1000000</v>
       </c>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40">
+      <c r="E29" s="37"/>
+      <c r="F29" s="37">
         <f t="shared" si="1"/>
         <v>5850950</v>
       </c>
-      <c r="G29" s="40">
+      <c r="G29" s="47">
+        <f t="shared" ref="G29:G44" si="7">(F29*15%)+F29</f>
+        <v>6728592.5</v>
+      </c>
+      <c r="H29" s="37">
         <f t="shared" si="6"/>
         <v>7313687.5</v>
       </c>
-      <c r="H29" s="40">
+      <c r="I29" s="37">
         <v>8500000</v>
       </c>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40">
+      <c r="J29" s="37"/>
+      <c r="K29" s="37">
         <f t="shared" si="4"/>
         <v>2649050</v>
       </c>
-      <c r="K29" s="41" t="s">
+      <c r="L29" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="N29" s="42" t="s">
+      <c r="O29" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="O29" s="41" t="s">
+      <c r="P29" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="P29" s="43">
+      <c r="Q29" s="40">
         <v>45019</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="56" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="66">
+    <row r="30" spans="1:18" s="53" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="63">
         <v>29</v>
       </c>
-      <c r="B30" s="54" t="s">
+      <c r="B30" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="55">
+      <c r="C30" s="52">
         <v>8317935</v>
       </c>
-      <c r="D30" s="55">
+      <c r="D30" s="52">
         <v>850000</v>
       </c>
-      <c r="E30" s="55"/>
-      <c r="F30" s="55">
+      <c r="E30" s="52"/>
+      <c r="F30" s="52">
         <f t="shared" si="1"/>
         <v>9167935</v>
       </c>
-      <c r="G30" s="55">
+      <c r="G30" s="47">
+        <f t="shared" si="7"/>
+        <v>10543125.25</v>
+      </c>
+      <c r="H30" s="52">
         <f t="shared" si="6"/>
         <v>11459918.75</v>
       </c>
-      <c r="H30" s="55">
+      <c r="I30" s="52">
         <v>9000000</v>
       </c>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55">
+      <c r="J30" s="52"/>
+      <c r="K30" s="52">
         <f t="shared" si="4"/>
         <v>-167935</v>
       </c>
-      <c r="K30" s="56" t="s">
+      <c r="L30" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="N30" s="57" t="s">
+      <c r="O30" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="O30" s="56" t="s">
+      <c r="P30" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="P30" s="58">
+      <c r="Q30" s="55">
         <v>45020</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="41" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="65">
+    <row r="31" spans="1:18" s="38" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="62">
         <v>30</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="40">
+      <c r="C31" s="37">
         <v>4258422</v>
       </c>
-      <c r="D31" s="40">
+      <c r="D31" s="37">
         <v>1064000</v>
       </c>
-      <c r="E31" s="40">
+      <c r="E31" s="37">
         <v>-1000000</v>
       </c>
-      <c r="F31" s="40">
+      <c r="F31" s="37">
         <f t="shared" si="1"/>
         <v>4322422</v>
       </c>
-      <c r="G31" s="40">
+      <c r="G31" s="47">
+        <f t="shared" si="7"/>
+        <v>4970785.3</v>
+      </c>
+      <c r="H31" s="37">
         <f t="shared" si="6"/>
         <v>5403027.5</v>
       </c>
-      <c r="H31" s="40">
+      <c r="I31" s="37">
         <v>5500000</v>
       </c>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40">
+      <c r="J31" s="37"/>
+      <c r="K31" s="37">
         <f t="shared" si="4"/>
         <v>1177578</v>
       </c>
-      <c r="K31" s="41" t="s">
+      <c r="L31" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="N31" s="42" t="s">
+      <c r="O31" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="O31" s="41" t="s">
+      <c r="P31" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="P31" s="43">
+      <c r="Q31" s="40">
         <v>45021</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="67">
+    <row r="32" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="64">
         <v>31</v>
       </c>
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="4">
         <v>6651048</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="4">
         <v>1300000</v>
       </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4">
         <f t="shared" si="1"/>
         <v>7951048</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="47">
+        <f t="shared" si="7"/>
+        <v>9143705.1999999993</v>
+      </c>
+      <c r="H32" s="4">
         <f t="shared" si="6"/>
         <v>9938810</v>
       </c>
-      <c r="H32" s="7" t="s">
+      <c r="I32" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7" t="e">
+      <c r="J32" s="4"/>
+      <c r="K32" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N32" s="18" t="s">
+      <c r="O32" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="O32" s="6" t="s">
+      <c r="P32" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P32" s="8">
+      <c r="Q32" s="5">
         <v>45022</v>
       </c>
     </row>
-    <row r="33" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="67">
+    <row r="33" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="64">
         <v>32</v>
       </c>
-      <c r="B33" s="68" t="s">
+      <c r="B33" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="4">
         <v>3558942</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="4">
         <v>2000000</v>
       </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7">
+      <c r="E33" s="4"/>
+      <c r="F33" s="4">
         <f t="shared" si="1"/>
         <v>5558942</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="47">
+        <f t="shared" si="7"/>
+        <v>6392783.2999999998</v>
+      </c>
+      <c r="H33" s="4">
         <f t="shared" si="6"/>
         <v>6948677.5</v>
       </c>
-      <c r="H33" s="7" t="s">
+      <c r="I33" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7" t="e">
+      <c r="J33" s="4"/>
+      <c r="K33" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N33" s="18" t="s">
+      <c r="O33" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="O33" s="6" t="s">
+      <c r="P33" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P33" s="8">
+      <c r="Q33" s="5">
         <v>45022</v>
       </c>
     </row>
-    <row r="34" spans="1:16" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="67">
+    <row r="34" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="64">
         <v>33</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="4">
         <v>9299103</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="4">
         <v>850000</v>
       </c>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7">
+      <c r="E34" s="4"/>
+      <c r="F34" s="4">
         <f t="shared" si="1"/>
         <v>10149103</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="47">
+        <f t="shared" si="7"/>
+        <v>11671468.449999999</v>
+      </c>
+      <c r="H34" s="4">
         <f t="shared" si="6"/>
         <v>12686378.75</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="I34" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7" t="e">
+      <c r="J34" s="4"/>
+      <c r="K34" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N34" s="18" t="s">
+      <c r="O34" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="O34" s="6" t="s">
+      <c r="P34" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P34" s="8">
+      <c r="Q34" s="5">
         <v>45027</v>
       </c>
     </row>
-    <row r="35" spans="1:16" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="67">
+    <row r="35" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="64">
         <v>34</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="4">
         <v>7849892</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="4">
         <v>1100000</v>
       </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7">
+      <c r="E35" s="4"/>
+      <c r="F35" s="4">
         <f t="shared" si="1"/>
         <v>8949892</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="47">
+        <f t="shared" si="7"/>
+        <v>10292375.800000001</v>
+      </c>
+      <c r="H35" s="4">
         <f t="shared" si="6"/>
         <v>11187365</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="I35" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7" t="e">
+      <c r="J35" s="4"/>
+      <c r="K35" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N35" s="18" t="s">
+      <c r="O35" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="O35" s="6" t="s">
+      <c r="P35" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="P35" s="8">
+      <c r="Q35" s="5">
         <v>45027</v>
       </c>
     </row>
-    <row r="36" spans="1:16" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="67">
+    <row r="36" spans="1:17" s="3" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="64">
         <v>35</v>
       </c>
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="4">
         <v>3972000</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="4">
         <v>850000</v>
       </c>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7">
+      <c r="E36" s="4"/>
+      <c r="F36" s="4">
         <f t="shared" si="1"/>
         <v>4822000</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="47">
+        <f t="shared" si="7"/>
+        <v>5545300</v>
+      </c>
+      <c r="H36" s="4">
         <f t="shared" si="6"/>
         <v>6027500</v>
       </c>
-      <c r="H36" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7" t="e">
+      <c r="I36" s="4">
+        <v>7000000</v>
+      </c>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4">
+        <f t="shared" si="4"/>
+        <v>2178000</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="O36" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q36" s="5"/>
+    </row>
+    <row r="37" spans="1:17" s="3" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="64">
+        <v>36</v>
+      </c>
+      <c r="B37" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="4">
+        <v>8467000</v>
+      </c>
+      <c r="D37" s="4">
+        <v>850000</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4">
+        <f t="shared" si="1"/>
+        <v>9317000</v>
+      </c>
+      <c r="G37" s="47">
+        <f t="shared" si="7"/>
+        <v>10714550</v>
+      </c>
+      <c r="H37" s="4">
+        <f t="shared" si="6"/>
+        <v>11646250</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N36" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="P36" s="8"/>
-    </row>
-    <row r="37" spans="1:16" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="67">
-        <v>36</v>
-      </c>
-      <c r="B37" s="69" t="s">
-        <v>94</v>
-      </c>
-      <c r="C37" s="7">
-        <v>8467000</v>
-      </c>
-      <c r="D37" s="7">
-        <v>850000</v>
-      </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7">
-        <f t="shared" si="1"/>
-        <v>9317000</v>
-      </c>
-      <c r="G37" s="7">
-        <f t="shared" si="6"/>
-        <v>11646250</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7" t="e">
+      <c r="O37" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q37" s="5"/>
+    </row>
+    <row r="38" spans="1:17" s="19" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="67">
+        <v>37</v>
+      </c>
+      <c r="B38" s="68" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="33">
+        <v>3178000</v>
+      </c>
+      <c r="D38" s="33">
+        <v>1220000</v>
+      </c>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33">
+        <f t="shared" si="1"/>
+        <v>4398000</v>
+      </c>
+      <c r="G38" s="47">
+        <f t="shared" si="7"/>
+        <v>5057700</v>
+      </c>
+      <c r="H38" s="4">
+        <f>(F38*25%)+F38</f>
+        <v>5497500</v>
+      </c>
+      <c r="I38" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="J38" s="33"/>
+      <c r="K38" s="33" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N37" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="P37" s="8"/>
-    </row>
-    <row r="38" spans="1:16" s="22" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="70">
-        <v>37</v>
-      </c>
-      <c r="B38" s="71" t="s">
-        <v>105</v>
-      </c>
-      <c r="C38" s="36">
-        <v>3178000</v>
-      </c>
-      <c r="D38" s="36">
-        <v>1220000</v>
-      </c>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36">
-        <f t="shared" si="1"/>
-        <v>4398000</v>
-      </c>
-      <c r="G38" s="7">
-        <f>(F38*25%)+F38</f>
-        <v>5497500</v>
-      </c>
-      <c r="H38" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36" t="e">
+      <c r="O38" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q38" s="34"/>
+    </row>
+    <row r="39" spans="1:17" s="3" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="67">
+        <v>38</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="31">
+        <v>4560000</v>
+      </c>
+      <c r="D39" s="33">
+        <v>850000</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4">
+        <f t="shared" si="1"/>
+        <v>5410000</v>
+      </c>
+      <c r="G39" s="47">
+        <f t="shared" si="7"/>
+        <v>6221500</v>
+      </c>
+      <c r="H39" s="4">
+        <f t="shared" si="6"/>
+        <v>6762500</v>
+      </c>
+      <c r="I39" s="4">
+        <v>7000000</v>
+      </c>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4">
+        <f t="shared" si="4"/>
+        <v>1590000</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="O39" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q39" s="24">
+        <v>45265</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="67">
+        <v>39</v>
+      </c>
+      <c r="B40" s="68" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="4">
+        <v>6156000</v>
+      </c>
+      <c r="D40" s="33">
+        <v>850000</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4">
+        <f t="shared" si="1"/>
+        <v>7006000</v>
+      </c>
+      <c r="G40" s="47">
+        <f t="shared" si="7"/>
+        <v>8056900</v>
+      </c>
+      <c r="H40" s="4">
+        <f t="shared" si="6"/>
+        <v>8757500</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N38" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="P38" s="37"/>
-    </row>
-    <row r="39" spans="1:16" s="6" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="70">
-        <v>38</v>
-      </c>
-      <c r="B39" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="C39" s="34">
-        <v>4560000</v>
-      </c>
-      <c r="D39" s="36">
+      <c r="O40" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q40" s="5"/>
+    </row>
+    <row r="41" spans="1:17" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="67">
+        <v>40</v>
+      </c>
+      <c r="B41" s="68" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="4">
+        <v>4126000</v>
+      </c>
+      <c r="D41" s="33">
         <v>850000</v>
       </c>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7">
-        <f t="shared" si="1"/>
-        <v>5410000</v>
-      </c>
-      <c r="G39" s="7">
+      <c r="E41" s="4"/>
+      <c r="F41" s="4">
+        <f t="shared" si="1"/>
+        <v>4976000</v>
+      </c>
+      <c r="G41" s="47">
+        <f t="shared" si="7"/>
+        <v>5722400</v>
+      </c>
+      <c r="H41" s="4">
         <f t="shared" si="6"/>
-        <v>6762500</v>
-      </c>
-      <c r="H39" s="7">
-        <v>7000000</v>
-      </c>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7">
-        <f t="shared" si="4"/>
-        <v>1590000</v>
-      </c>
-      <c r="K39" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="N39" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="P39" s="27">
-        <v>45265</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="70">
-        <v>39</v>
-      </c>
-      <c r="B40" s="71" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" s="7">
-        <v>6156000</v>
-      </c>
-      <c r="D40" s="36">
-        <v>850000</v>
-      </c>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7">
-        <f t="shared" si="1"/>
-        <v>7006000</v>
-      </c>
-      <c r="G40" s="7">
-        <f t="shared" si="6"/>
-        <v>8757500</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7" t="e">
+        <v>6220000</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N40" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="P40" s="8"/>
-    </row>
-    <row r="41" spans="1:16" s="6" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="70">
-        <v>40</v>
-      </c>
-      <c r="B41" s="71" t="s">
-        <v>108</v>
-      </c>
-      <c r="C41" s="7">
-        <v>4126000</v>
-      </c>
-      <c r="D41" s="36">
+      <c r="O41" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q41" s="5"/>
+    </row>
+    <row r="42" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="67">
+        <v>41</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="31">
+        <v>3192000</v>
+      </c>
+      <c r="D42" s="33">
         <v>850000</v>
       </c>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7">
-        <f t="shared" si="1"/>
-        <v>4976000</v>
-      </c>
-      <c r="G41" s="7">
+      <c r="E42" s="4"/>
+      <c r="F42" s="4">
+        <f t="shared" si="1"/>
+        <v>4042000</v>
+      </c>
+      <c r="G42" s="47">
+        <f t="shared" si="7"/>
+        <v>4648300</v>
+      </c>
+      <c r="H42" s="4">
         <f t="shared" si="6"/>
-        <v>6220000</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7" t="e">
+        <v>5052500</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N41" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="P41" s="8"/>
-    </row>
-    <row r="42" spans="1:16" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="70">
-        <v>41</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="C42" s="34">
-        <v>3192000</v>
-      </c>
-      <c r="D42" s="36">
+      <c r="O42" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q42" s="24"/>
+    </row>
+    <row r="43" spans="1:17" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="67">
+        <v>42</v>
+      </c>
+      <c r="B43" s="66" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="31">
+        <v>6065000</v>
+      </c>
+      <c r="D43" s="4">
         <v>850000</v>
       </c>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7">
-        <f t="shared" si="1"/>
-        <v>4042000</v>
-      </c>
-      <c r="G42" s="7">
+      <c r="E43" s="4"/>
+      <c r="F43" s="4">
+        <f t="shared" si="1"/>
+        <v>6915000</v>
+      </c>
+      <c r="G43" s="47">
+        <f t="shared" si="7"/>
+        <v>7952250</v>
+      </c>
+      <c r="H43" s="4">
         <f t="shared" si="6"/>
-        <v>5052500</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7" t="e">
+        <v>8643750</v>
+      </c>
+      <c r="I43" s="4">
+        <v>8500000</v>
+      </c>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4">
+        <f t="shared" si="4"/>
+        <v>1585000</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="O43" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q43" s="24"/>
+    </row>
+    <row r="44" spans="1:17" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="67">
+        <v>43</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" s="31">
+        <v>3268000</v>
+      </c>
+      <c r="D44" s="4">
+        <v>850000</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4">
+        <f t="shared" si="1"/>
+        <v>4118000</v>
+      </c>
+      <c r="G44" s="47">
+        <f t="shared" si="7"/>
+        <v>4735700</v>
+      </c>
+      <c r="H44" s="4">
+        <f t="shared" si="6"/>
+        <v>5147500</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N42" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="P42" s="27"/>
-    </row>
-    <row r="43" spans="1:16" s="6" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="70">
-        <v>42</v>
-      </c>
-      <c r="B43" s="69" t="s">
-        <v>112</v>
-      </c>
-      <c r="C43" s="34">
-        <v>6065000</v>
-      </c>
-      <c r="D43" s="7">
-        <v>850000</v>
-      </c>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7">
-        <f t="shared" si="1"/>
-        <v>6915000</v>
-      </c>
-      <c r="G43" s="7">
-        <f t="shared" si="6"/>
-        <v>8643750</v>
-      </c>
-      <c r="H43" s="7">
-        <v>8500000</v>
-      </c>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7">
-        <f t="shared" si="4"/>
-        <v>1585000</v>
-      </c>
-      <c r="K43" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="N43" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="P43" s="27"/>
-    </row>
-    <row r="44" spans="1:16" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="70">
-        <v>43</v>
-      </c>
-      <c r="B44" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="C44" s="34">
-        <v>3268000</v>
-      </c>
-      <c r="D44" s="7">
-        <v>850000</v>
-      </c>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7">
-        <f t="shared" si="1"/>
-        <v>4118000</v>
-      </c>
-      <c r="G44" s="7">
-        <f t="shared" si="6"/>
-        <v>5147500</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="N44" s="73" t="s">
+      <c r="O44" s="70" t="s">
         <v>120</v>
       </c>
-      <c r="O44" s="27"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" s="29">
+      <c r="P44" s="24"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="26">
         <v>40</v>
       </c>
-      <c r="B45" s="30"/>
-      <c r="C45" s="35"/>
-      <c r="J45" s="72"/>
-      <c r="N45" s="32"/>
-      <c r="P45" s="33"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
-      <c r="C46" s="35"/>
-      <c r="N46" s="32"/>
-      <c r="P46" s="33"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J47" s="3">
+      <c r="B45" s="27"/>
+      <c r="C45" s="32"/>
+      <c r="K45" s="69"/>
+      <c r="O45" s="29"/>
+      <c r="Q45" s="30"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="26"/>
+      <c r="C46" s="32"/>
+      <c r="O46" s="29"/>
+      <c r="Q46" s="30"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K47" s="2">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C48" s="3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
         <f>SUM(C2:C8)</f>
         <v>46150000</v>
       </c>
-      <c r="H48" s="3">
-        <f>SUM(H2:H8)</f>
+      <c r="I48" s="2">
+        <f>SUM(I2:I8)</f>
         <v>50200000</v>
       </c>
-      <c r="J48" s="3">
+      <c r="K48" s="2">
         <f t="shared" si="4"/>
         <v>50200000</v>
       </c>
-      <c r="L48" t="s">
+      <c r="M48" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="3">
+      <c r="D52" s="2">
         <f>SUM(C20:C25)</f>
         <v>37301557</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="K1:K52" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="C2:F2 G2:M17 N2:P22 B2:B25 Q2:Q39 C3:E25 F3:F38 J3:J38 G18:I35 K18:M38 O23:P25 N26:P26 D26:E38 O26:O39 C29:E38 N29:P38 H36:I38 G36:G42 D39:F39 H39:M39 C40:F41 H40:Q41 H42:I42 O42:O43 Q42:Q43 K42:M46 J42:J48 P44 O45:O46 Q45:Q46 D42:F42 D43:I46">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <autoFilter ref="L1:L52" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="C2:G2 H2:N17 O2:Q22 B2:B25 R2:R39 C3:E25 F3:G28 K3:K38 H18:J35 L18:N38 P23:Q25 O26:Q26 D26:E38 P26:P39 O29:Q38 I36:J38 H36:H42 D39:F39 I39:N39 C40:F41 I40:R41 I42:J42 P42:P43 R42:R43 L42:N46 K42:K48 Q44 P45:P46 R45:R46 D45:J46 D42:F44 H43:J44 C29:F38 G29:G44">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>MOD(ROW(),2)&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="N23" r:id="rId1" display="https://www.ebay.com/ship/trk/tracking-details?transid=2201839708010&amp;itemid=204283961060" xr:uid="{6F8BFF36-4018-4EC5-AB4D-4659A4D8A44B}"/>
+    <hyperlink ref="O23" r:id="rId1" display="https://www.ebay.com/ship/trk/tracking-details?transid=2201839708010&amp;itemid=204283961060" xr:uid="{6F8BFF36-4018-4EC5-AB4D-4659A4D8A44B}"/>
     <hyperlink ref="B26" r:id="rId2" display="https://www.ebay.com/itm/334809987318" xr:uid="{19E8C091-88D6-4919-B8E7-96C96784B012}"/>
-    <hyperlink ref="N24" r:id="rId3" display="https://www.ebay.com/ship/trk/tracking-details?transid=0&amp;itemid=394522922692" xr:uid="{33A4F9FB-78A6-4311-9764-2BC4A4E1AFF3}"/>
+    <hyperlink ref="O24" r:id="rId3" display="https://www.ebay.com/ship/trk/tracking-details?transid=0&amp;itemid=394522922692" xr:uid="{33A4F9FB-78A6-4311-9764-2BC4A4E1AFF3}"/>
     <hyperlink ref="B29" r:id="rId4" display="https://www.ebay.com/itm/314434790481" xr:uid="{85980ED6-45D8-4091-8276-909E0D9EE162}"/>
     <hyperlink ref="B33" r:id="rId5" display="https://www.ebay.com/itm/256028369435" xr:uid="{C70628C0-D734-4DC0-963A-20DE1823E713}"/>
     <hyperlink ref="B37" r:id="rId6" display="https://www.ebay.com/itm/175682167857" xr:uid="{7381F593-AD6B-483E-BEA5-4F4B3E158710}"/>
@@ -2981,168 +3199,242 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3777B8E6-A987-471D-8EED-3DECBE1A9A65}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18" style="5" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="74.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="75" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>34534861886</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="5">
-        <v>44835</v>
-      </c>
-      <c r="D2" s="3">
-        <v>6700000</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="3">
-        <f>(D2*15%)+D2</f>
-        <v>7705000</v>
-      </c>
-      <c r="G2" s="3">
-        <f xml:space="preserve"> D2+200000</f>
-        <v>6900000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="5">
-        <v>44841</v>
-      </c>
-      <c r="D3" s="3">
-        <v>4900000</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="3">
-        <f>(D3*15%)+D3</f>
-        <v>5635000</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ref="G3:G7" si="0" xml:space="preserve"> D3+200000</f>
-        <v>5100000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="5">
-        <v>44841</v>
-      </c>
-      <c r="D4" s="3">
-        <v>6700000</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="3">
-        <f t="shared" ref="F4" si="1">(D4*15%)+D4</f>
-        <v>7705000</v>
-      </c>
-      <c r="G4" s="3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="4">
+        <v>7951048</v>
+      </c>
+      <c r="D2" s="47">
+        <f>(C2*15%)+C2</f>
+        <v>9143705.1999999993</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="77" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="4">
+        <v>5558942</v>
+      </c>
+      <c r="D3" s="47">
+        <f t="shared" ref="D3:D10" si="0">(C3*15%)+C3</f>
+        <v>6392783.2999999998</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="72" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="4">
+        <v>10149103</v>
+      </c>
+      <c r="D4" s="47">
         <f t="shared" si="0"/>
-        <v>6900000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="5">
-        <v>44845</v>
-      </c>
-      <c r="D6" s="3">
-        <v>7500000</v>
-      </c>
-      <c r="F6" s="3">
-        <f t="shared" ref="F6:F7" si="2">(D6*15%)+D6</f>
-        <v>8625000</v>
-      </c>
-      <c r="G6" s="3">
+        <v>11671468.449999999</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="72" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="4">
+        <v>8949892</v>
+      </c>
+      <c r="D5" s="47">
         <f t="shared" si="0"/>
-        <v>7700000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="5">
-        <v>44876</v>
-      </c>
-      <c r="D7" s="3">
-        <v>11500000</v>
-      </c>
-      <c r="F7" s="3">
-        <f t="shared" si="2"/>
-        <v>13225000</v>
-      </c>
-      <c r="G7" s="3">
+        <v>10292375.800000001</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="33">
+        <v>4398000</v>
+      </c>
+      <c r="D6" s="47">
         <f t="shared" si="0"/>
-        <v>11700000</v>
-      </c>
+        <v>5057700</v>
+      </c>
+      <c r="E6" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="68" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="4">
+        <v>7006000</v>
+      </c>
+      <c r="D7" s="47">
+        <f t="shared" si="0"/>
+        <v>8056900</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="4">
+        <v>4976000</v>
+      </c>
+      <c r="D8" s="47">
+        <f t="shared" si="0"/>
+        <v>5722400</v>
+      </c>
+      <c r="E8" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="4">
+        <v>4042000</v>
+      </c>
+      <c r="D9" s="47">
+        <f t="shared" si="0"/>
+        <v>4648300</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="77" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="4">
+        <v>4118000</v>
+      </c>
+      <c r="D10" s="47">
+        <f t="shared" si="0"/>
+        <v>4735700</v>
+      </c>
+      <c r="E10" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="76"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="28"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C10 D2:E11">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>MOD(ROW(),2)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>MOD(ROW(),2)&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>